<commit_message>
Added materials required for AWRA conference
</commit_message>
<xml_diff>
--- a/03.outputs/final_modified.xlsx
+++ b/03.outputs/final_modified.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bama365-my.sharepoint.com/personal/snaserneisary_crimson_ua_edu/Documents/02.projects/02.nidis/02.code/nrt-nwm-benchmark-project/03.outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_23F921ED6F734E6B0565401671318F70412498D9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0644694F-287D-43E7-B1FA-A48D3D23EDF6}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_23F921ED6F734E6B0565401671318F70412498D9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAF051CB-EAC9-264C-A875-020B43927E03}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -400,6 +400,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -692,15 +696,17 @@
   <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,7 +792,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -869,7 +875,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -952,7 +958,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>17</v>
       </c>
@@ -1035,7 +1041,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>18</v>
       </c>
@@ -1118,7 +1124,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1201,7 +1207,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -1284,7 +1290,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -1367,7 +1373,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -1450,7 +1456,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1533,7 +1539,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -1616,7 +1622,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1699,7 +1705,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -1782,7 +1788,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -1865,7 +1871,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>7</v>
       </c>
@@ -1948,7 +1954,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>11</v>
       </c>
@@ -2031,7 +2037,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>12</v>
       </c>
@@ -2114,7 +2120,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>14</v>
       </c>
@@ -2197,7 +2203,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>13</v>
       </c>
@@ -2280,7 +2286,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>15</v>
       </c>

</xml_diff>